<commit_message>
add gender and tissue samples to mactaquac tagging
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-pit_tagging.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-pit_tagging.xlsx
@@ -168,13 +168,26 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t>Optional, units can be set to either (mm) or (cm)</t>
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="O3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Vial Number</t>
   </si>
@@ -269,6 +282,9 @@
   </si>
   <si>
     <t>Tissue Sample</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -304,7 +320,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +330,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,7 +365,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,18 +664,18 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -694,28 +703,31 @@
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update units in tagging parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-pit_tagging.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-pit_tagging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED02B96A-5F9A-4968-8A79-853674ADBC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62B80E-3892-485E-92B8-AD7830F835EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Weight (kg)</t>
-  </si>
-  <si>
-    <t>Length (mm)</t>
-  </si>
-  <si>
     <t>UFID</t>
   </si>
   <si>
@@ -139,6 +133,12 @@
   </si>
   <si>
     <t>Fill in if a movement occurred, or if origin tank is unknown. E.g. LP1</t>
+  </si>
+  <si>
+    <t>Length (cm)</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A2:RU3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,13 +570,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>8</v>
@@ -594,22 +594,22 @@
         <v>5</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="P2" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>4</v>
@@ -617,64 +617,64 @@
     </row>
     <row r="3" spans="1:489" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="T3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>

</xml_diff>